<commit_message>
Add more Web Scraping ideas
</commit_message>
<xml_diff>
--- a/Diena_15_Web_Scraping/riga_center_60.xlsx
+++ b/Diena_15_Web_Scraping/riga_center_60.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="251">
   <si>
     <t>Sludinājumi 	datums</t>
   </si>
@@ -46,6 +46,126 @@
     <t>Cena</t>
   </si>
   <si>
+    <t>3 istabu dzīvoklis Viktora Štama projektētā jūgendstila namā.</t>
+  </si>
+  <si>
+    <t>Laba cena par dzīvokli izcilā vietā. Panorāmas skats no logiem</t>
+  </si>
+  <si>
+    <t>Izbaudiet Rīgas pilsētas dzīvi, atrodoties tās epicentrā - iegād</t>
+  </si>
+  <si>
+    <t>Наслаждайся прелестями городской жизни, находять в ее эпицентре</t>
+  </si>
+  <si>
+    <t>Продается просторная, солнечная с изолированными комнатами кварт</t>
+  </si>
+  <si>
+    <t>Īpašnieks pārdod izremontētu, mēbelētu, gaišu dzīvokli Rīgas cen</t>
+  </si>
+  <si>
+    <t>Divu istabu, ar ērtu plānojumu dzīvoklis, ēkas piektajā stāvā, i</t>
+  </si>
+  <si>
+    <t>Pārdodu 3-istabu dzīvokli Vesetas ielā 8, vienā no labākajiem sp</t>
+  </si>
+  <si>
+    <t>3 комнатная квартира в новом проекте Futuris, полностью мебелиро</t>
+  </si>
+  <si>
+    <t>Plašs divu līmeņu dzīvoklis Rīgas centrā ar terasi. Brīnišķ</t>
+  </si>
+  <si>
+    <t>Iebūvēta privātmāja Rīgas centrā ar privāto terasi. Brīnišķ</t>
+  </si>
+  <si>
+    <t>Pārdod mūsdienīgu, gaišu un plašu dzīvokli renovētā dzīvojamā mā</t>
+  </si>
+  <si>
+    <t>Pārdod modernu un mājīgu 2-istabu dzīvokli Brīvības ielā pie Cēs</t>
+  </si>
+  <si>
+    <t>Skaists un gaumīgs 4-istabu dzīvoklis renovētā mājā blakus parka</t>
+  </si>
+  <si>
+    <t>В новом проекте Lofts&amp;rosegold продаём пятикомнатную квартиру со</t>
+  </si>
+  <si>
+    <t>В новом проекте Lofts&amp;rosegold продаём двухкомнатную квартиру с</t>
+  </si>
+  <si>
+    <t>Хозяин продаёт квартиру в тихом центре. Квартира состоит из</t>
+  </si>
+  <si>
+    <t>Īpašnieks samazina cenu un pārdod dzīvokli ar pēlēko apdari reno</t>
+  </si>
+  <si>
+    <t>Стильная и уютная квартира в центре Риги, высокий первый этаж. К</t>
+  </si>
+  <si>
+    <t>Застройщик предлагает Studio квартиру в полностью реконструирова</t>
+  </si>
+  <si>
+    <t>Аренда с правом выкупа. Застройщик предлагает студио типа кв</t>
+  </si>
+  <si>
+    <t>Trīs istabas izolētas kapitālais remonts, studio tipa istaba, ap</t>
+  </si>
+  <si>
+    <t>Земля в собственности + бесплатный паркинг у дома - бонус для кр</t>
+  </si>
+  <si>
+    <t>Уютно , спокойно , красиво , качественно и стабильно , а ещё оче</t>
+  </si>
+  <si>
+    <t>Земля в собственности - В самом центре Риги, рядом с красивым па</t>
+  </si>
+  <si>
+    <t>Saimnieks pārdod lielisku trīs istabu dzīvokli ar kopējo platību</t>
+  </si>
+  <si>
+    <t>Pārdod dzīvokli centrā Elku ielā. Dzīvoklis atrodas renovētas ēk</t>
+  </si>
+  <si>
+    <t>Īpašnieks pārdod tīru, gaišu, siltu 1-ist. dzīvokli pēc mūsdienī</t>
+  </si>
+  <si>
+    <t>Pārdod bez starpniekiem plašu dzīvokli, augstie griesti , 3 ista</t>
+  </si>
+  <si>
+    <t>Nekustamā īpašuma trīs zelta likumi. -Vieta, -Vieta un -Vi</t>
+  </si>
+  <si>
+    <t>Pārdod īpašumu pašā Rīgas centra sirdī. -Skandināvu stilā iekā</t>
+  </si>
+  <si>
+    <t>Квартира с панорамными окнами и прекрасным видом на Межапарк. Те</t>
+  </si>
+  <si>
+    <t>Īpašnieks pārdod lielisku dzīvokli, labā stāvoklī, labā vietā-fa</t>
+  </si>
+  <si>
+    <t>Eleganta , komfortabla četrustāvu māja Rīgas vēsturiskajā centrā</t>
+  </si>
+  <si>
+    <t>Pārdodu mājīgu 2 istabu studio tipa dzīvokli, vēsturiskā (pirms</t>
+  </si>
+  <si>
+    <t>Pārdod dzīvokli centrā, klusā, zaļā vietā, Ieroču ielā. Dzīvok</t>
+  </si>
+  <si>
+    <t>Pārdodu vienistabas dzīvokli ar 3, 40 m augstiem griestiem. At</t>
+  </si>
+  <si>
+    <t>Plašs dzīvoklis Rīgas centrāar zemi īpašumā. Mājā ir lifts. Dzīv</t>
+  </si>
+  <si>
+    <t>Gaišs iekšpagalms. Pārdod dzīvokli ar jauniem stāvvadiem, jauna</t>
+  </si>
+  <si>
+    <t>Pārdod studio tipa dzīvokli renovētā mājā. Pvn iekļauts cenā.</t>
+  </si>
+  <si>
     <t>Īpašnieks pārdod dzīvokli renovētā namā Rīgas centrā. Dzīvokļa l</t>
   </si>
   <si>
@@ -79,121 +199,115 @@
     <t>Lielisks novietojums, saprātīga cena. Pagalma māja ar ieeju no</t>
   </si>
   <si>
-    <t>Сниженная цена. Тихий дом, памятник архитектуры, в ближайшее вре</t>
-  </si>
-  <si>
-    <t>5 izolētas istabas, atsevišķa virtuve, 2 san/mezgli. Griestu a</t>
-  </si>
-  <si>
-    <t>Pārdod saulainu un plašu dzīvokli klusā vietā Rīgas centrā. I</t>
-  </si>
-  <si>
-    <t>Ar gāzes apkuri, 1.augstais stāvs, reāli kā otrais stāvs. Dzīv</t>
-  </si>
-  <si>
-    <t>Mēbelēts dzīvoklis klasiska stila piekritējiem. Atrašanās vieta</t>
-  </si>
-  <si>
-    <t>Vienistabas dzīvoklis atrodas atjaunotā trīs ēku kompleksā "Rēde</t>
-  </si>
-  <si>
-    <t>Jauna cena. Kvalitatīvs dzīvoklis specprojekta mājā. Atsevišķa m</t>
-  </si>
-  <si>
-    <t>Pārdod trīsistabu dzīvokli "Skanstes virsotnēs" ar burvīgu skatu</t>
-  </si>
-  <si>
-    <t>Jauna cena. Ekskluzīvs dzīvoklis ar skatu uz parku jaunajā proje</t>
-  </si>
-  <si>
-    <t>Pārdodu plašu 5 istabu dzīvokli projektā „Šokolāde” (2008). Papi</t>
-  </si>
-  <si>
-    <t>Tiek piedāvāts renovēts divu līmeņu 3 istabu mansarda dzīvoklis</t>
-  </si>
-  <si>
-    <t>Просторная и продуманная квартира в новом проекте. Тщательно</t>
-  </si>
-  <si>
-    <t>Pārdodas ļoti kluss un gaišs 3.5 istabu dzīvoklis Rīgas centrā.</t>
-  </si>
-  <si>
-    <t>Saimnieks pārdod 3-istabu dzīvokli ļoti labā atrašanās vietā. Dz</t>
-  </si>
-  <si>
-    <t>Pārdodas 1-istabas dzīvoklis parastajā stāvokli. Dzīvoklim viena</t>
-  </si>
-  <si>
-    <t>Jaunums. Vienīgais mazizmēra dzīvoklis, kurš pārdodās Hospitāļu</t>
-  </si>
-  <si>
-    <t>Īpašnieks samazina cenu un pārdod dzīvokli ar pēlēko apdari reno</t>
-  </si>
-  <si>
-    <t>Уютная и удобная квартира в фасадном доме 1908 года постройки. О</t>
-  </si>
-  <si>
-    <t>Tiešais saimnieks. Ar visām mēbelēm. Bez komisijas maksas. Vai</t>
-  </si>
-  <si>
-    <t>Pārdodu labu tris istabu dzīvokli centrā. Dzīvoklim ir krāsns ap</t>
-  </si>
-  <si>
-    <t>Фасадный дом, окна выходят на обе стороны. Уютная и удобная квар</t>
-  </si>
-  <si>
-    <t>Piedāvājumā ir pieejams pilnībā renovēts dzīvoklis 1939. gadā ce</t>
-  </si>
-  <si>
-    <t>Autostāvvieta iekļauta cenā ( 8000€ vērtībā) + Virtuve iekļauta</t>
-  </si>
-  <si>
-    <t>Стильная и комфортная квартира в современном проекте Skanstes Pa</t>
-  </si>
-  <si>
-    <t>Plašs trīsistabu dzīvokli renovētā pirmskara mājā, ļoti labā atr</t>
-  </si>
-  <si>
-    <t>Pārdodam 2 istabu dzīvokli Rīgas centrā, renovēta māja. Platība</t>
-  </si>
-  <si>
-    <t>Pārdod plašu dzīvokli Rīgas Centrā Tiek piedāvāts dzīvoklis R</t>
-  </si>
-  <si>
-    <t>Pārdod tikko kapitāli remontētu 3 istabu dzīvokli ar visu nepiec</t>
-  </si>
-  <si>
-    <t>Pārdod remontētu vienas istabas dzīvokli. Vieta automašīnai ēkas</t>
-  </si>
-  <si>
-    <t>Dizainera veidota apdare, pilnībā mēbelēts, stilīgs 2-līmeņu man</t>
-  </si>
-  <si>
-    <t>Продается полуподвальное помещение (с окном и высокими арочными</t>
-  </si>
-  <si>
-    <t>Centrs. Klusa un mierīga vieta, zems trokšņu līmenis. Laba vie</t>
-  </si>
-  <si>
-    <t>Pārdod gaišu studiju jaunajā projektā Klusā ielā. Māja nodota ek</t>
-  </si>
-  <si>
-    <t>Lat/rus/ Virtuves mēbēles davanā no attistītāja. Dzīvoklis ar pi</t>
-  </si>
-  <si>
-    <t>Lat/rus Labākais renovācijas projekts 2019. gadā - Gada balva.</t>
-  </si>
-  <si>
-    <t>Lat/rus. Kompakts(59m2) 3.ist. dzīvoklis. Labākais renovācijas p</t>
-  </si>
-  <si>
-    <t>Pārdodam elegantu 5 istabu dzīvokli pilsētas centrā. Dizainera v</t>
-  </si>
-  <si>
-    <t>Lielisks dzīvoklis pašā Rīgas sirdī. Veikts kapitālais remonts,</t>
-  </si>
-  <si>
-    <t>Pārdod skaistu un mājīgu, maz izmantotu dzīvokli jaunajā projekt</t>
+    <t>Gogoļa 10</t>
+  </si>
+  <si>
+    <t>Teātra 12</t>
+  </si>
+  <si>
+    <t>Dzirnavu 83</t>
+  </si>
+  <si>
+    <t>Dzirnavu 81</t>
+  </si>
+  <si>
+    <t>Zaļā 4</t>
+  </si>
+  <si>
+    <t>Lāčplēša 52</t>
+  </si>
+  <si>
+    <t>Klijānu 6</t>
+  </si>
+  <si>
+    <t>Vesetas 8</t>
+  </si>
+  <si>
+    <t>Antonijas 16A</t>
+  </si>
+  <si>
+    <t>Indrānu 8</t>
+  </si>
+  <si>
+    <t>Indrānu 5</t>
+  </si>
+  <si>
+    <t>Cēsu 23</t>
+  </si>
+  <si>
+    <t>Brīvības 165</t>
+  </si>
+  <si>
+    <t>Klusā 11</t>
+  </si>
+  <si>
+    <t>Strēlnieku 8</t>
+  </si>
+  <si>
+    <t>Rūpniecības 16/2</t>
+  </si>
+  <si>
+    <t>Merķeļa 7</t>
+  </si>
+  <si>
+    <t>Cēsu 43</t>
+  </si>
+  <si>
+    <t>Lāčplēša 24</t>
+  </si>
+  <si>
+    <t>Birznieka-Upīša 10</t>
+  </si>
+  <si>
+    <t>Stabu 60</t>
+  </si>
+  <si>
+    <t>Ausekļa 8</t>
+  </si>
+  <si>
+    <t>Ģertrūdes 91</t>
+  </si>
+  <si>
+    <t>Pulkv. Brieža 13</t>
+  </si>
+  <si>
+    <t>Elku 4</t>
+  </si>
+  <si>
+    <t>Tallinas 75A</t>
+  </si>
+  <si>
+    <t>Matīsa 89a</t>
+  </si>
+  <si>
+    <t>Blaumaņa 26</t>
+  </si>
+  <si>
+    <t>Stabu 20</t>
+  </si>
+  <si>
+    <t>Duntes 28</t>
+  </si>
+  <si>
+    <t>Klusā 18</t>
+  </si>
+  <si>
+    <t>Skolas 36a</t>
+  </si>
+  <si>
+    <t>Klusā 9</t>
+  </si>
+  <si>
+    <t>Ieroču 10</t>
+  </si>
+  <si>
+    <t>Kazarmu 3a</t>
+  </si>
+  <si>
+    <t>Brīvības 150</t>
+  </si>
+  <si>
+    <t>Brīvības 39a</t>
   </si>
   <si>
     <t>Avotu 4</t>
@@ -217,9 +331,6 @@
     <t>Čaka 105</t>
   </si>
   <si>
-    <t>Duntes 28</t>
-  </si>
-  <si>
     <t>Miera 5</t>
   </si>
   <si>
@@ -229,211 +340,217 @@
     <t>Tērbatas 41/43</t>
   </si>
   <si>
-    <t>Antonijas 15</t>
-  </si>
-  <si>
-    <t>Elijas 5</t>
-  </si>
-  <si>
-    <t>Indrānu 21</t>
-  </si>
-  <si>
-    <t>Maskavas 22</t>
-  </si>
-  <si>
-    <t>Eksporta 8</t>
-  </si>
-  <si>
-    <t>Maskavas 48</t>
-  </si>
-  <si>
-    <t>Sadovņikova 21</t>
-  </si>
-  <si>
-    <t>Skanstes 29A</t>
-  </si>
-  <si>
-    <t>Rūpniecības 21</t>
-  </si>
-  <si>
-    <t>Hospitāļu 23</t>
-  </si>
-  <si>
-    <t>Valdemāra 57/59</t>
-  </si>
-  <si>
-    <t>Brīvības 230</t>
-  </si>
-  <si>
-    <t>Stabu 57</t>
-  </si>
-  <si>
-    <t>Stabu 29</t>
-  </si>
-  <si>
-    <t>Ganību d. 15</t>
-  </si>
-  <si>
-    <t>Hospitāļu 3</t>
-  </si>
-  <si>
-    <t>Merķeļa 7</t>
-  </si>
-  <si>
-    <t>Ģertrūdes 26</t>
-  </si>
-  <si>
-    <t>Ģertrūdes 91</t>
-  </si>
-  <si>
-    <t>Pērnavas 43</t>
-  </si>
-  <si>
-    <t>Ģertrūdes 99</t>
-  </si>
-  <si>
-    <t>Vesetas 15</t>
-  </si>
-  <si>
-    <t>Ausekļa 2</t>
-  </si>
-  <si>
-    <t>Valdemāra 11</t>
-  </si>
-  <si>
-    <t>Stabu 60</t>
-  </si>
-  <si>
-    <t>Cēsu 43</t>
-  </si>
-  <si>
-    <t>Sadovņikova 23</t>
-  </si>
-  <si>
-    <t>Baznīcas 13</t>
-  </si>
-  <si>
-    <t>Visvalža 3B</t>
-  </si>
-  <si>
-    <t>Klusā 20</t>
-  </si>
-  <si>
-    <t>Avotu 5</t>
-  </si>
-  <si>
-    <t>Čaka 26</t>
-  </si>
-  <si>
-    <t>Marijas 16</t>
-  </si>
-  <si>
-    <t>Blaumaņa 36</t>
-  </si>
-  <si>
-    <t>Klijānu 6</t>
+    <t>2/5</t>
+  </si>
+  <si>
+    <t>6/7</t>
+  </si>
+  <si>
+    <t>4/7</t>
+  </si>
+  <si>
+    <t>7/7</t>
   </si>
   <si>
     <t>5/5</t>
   </si>
   <si>
+    <t>5/9</t>
+  </si>
+  <si>
+    <t>5/7</t>
+  </si>
+  <si>
+    <t>1/5</t>
+  </si>
+  <si>
+    <t>2/6</t>
+  </si>
+  <si>
+    <t>5/6</t>
+  </si>
+  <si>
+    <t>3/5</t>
+  </si>
+  <si>
+    <t>4/5</t>
+  </si>
+  <si>
+    <t>4/6</t>
+  </si>
+  <si>
+    <t>3/6</t>
+  </si>
+  <si>
+    <t>1/6</t>
+  </si>
+  <si>
+    <t>3/3</t>
+  </si>
+  <si>
+    <t>6/6</t>
+  </si>
+  <si>
+    <t>11/16</t>
+  </si>
+  <si>
+    <t>3/9</t>
+  </si>
+  <si>
+    <t>2/4</t>
+  </si>
+  <si>
+    <t>3/4</t>
+  </si>
+  <si>
     <t>4/4</t>
   </si>
   <si>
-    <t>4/6</t>
-  </si>
-  <si>
-    <t>2/6</t>
-  </si>
-  <si>
-    <t>6/6</t>
-  </si>
-  <si>
-    <t>5/6</t>
-  </si>
-  <si>
-    <t>1/5</t>
-  </si>
-  <si>
     <t>2/2</t>
   </si>
   <si>
     <t>3/16</t>
   </si>
   <si>
-    <t>2/5</t>
-  </si>
-  <si>
-    <t>4/5</t>
-  </si>
-  <si>
-    <t>3/3</t>
-  </si>
-  <si>
-    <t>1/2</t>
-  </si>
-  <si>
-    <t>12/24</t>
-  </si>
-  <si>
-    <t>4/7</t>
-  </si>
-  <si>
-    <t>5/8</t>
-  </si>
-  <si>
-    <t>7/7</t>
-  </si>
-  <si>
-    <t>6/10</t>
-  </si>
-  <si>
-    <t>1/6</t>
-  </si>
-  <si>
-    <t>3/6</t>
-  </si>
-  <si>
-    <t>3/5</t>
-  </si>
-  <si>
-    <t>3/4</t>
-  </si>
-  <si>
-    <t>2/3</t>
-  </si>
-  <si>
-    <t>1/4</t>
-  </si>
-  <si>
-    <t>3/9</t>
-  </si>
-  <si>
-    <t>1/7</t>
-  </si>
-  <si>
-    <t>2/9</t>
+    <t>P. kara</t>
+  </si>
+  <si>
+    <t>Jaun.</t>
+  </si>
+  <si>
+    <t>Specpr.</t>
   </si>
   <si>
     <t>Renov.</t>
   </si>
   <si>
+    <t>Staļina</t>
+  </si>
+  <si>
     <t>Hrušč.</t>
   </si>
   <si>
-    <t>P. kara</t>
-  </si>
-  <si>
-    <t>Jaun.</t>
-  </si>
-  <si>
     <t>Priv. m.</t>
   </si>
   <si>
-    <t>Specpr.</t>
-  </si>
-  <si>
-    <t>Staļina</t>
+    <t>1,257 €</t>
+  </si>
+  <si>
+    <t>2,022 €</t>
+  </si>
+  <si>
+    <t>3,750 €</t>
+  </si>
+  <si>
+    <t>3,167 €</t>
+  </si>
+  <si>
+    <t>1,649 €</t>
+  </si>
+  <si>
+    <t>3,000 €</t>
+  </si>
+  <si>
+    <t>1,500 €</t>
+  </si>
+  <si>
+    <t>1,610 €</t>
+  </si>
+  <si>
+    <t>3,486 €</t>
+  </si>
+  <si>
+    <t>1,305 €</t>
+  </si>
+  <si>
+    <t>1,756 €</t>
+  </si>
+  <si>
+    <t>1,695 €</t>
+  </si>
+  <si>
+    <t>1,944 €</t>
+  </si>
+  <si>
+    <t>2,206 €</t>
+  </si>
+  <si>
+    <t>2,593 €</t>
+  </si>
+  <si>
+    <t>2,346 €</t>
+  </si>
+  <si>
+    <t>1,879 €</t>
+  </si>
+  <si>
+    <t>1,708 €</t>
+  </si>
+  <si>
+    <t>1,333 €</t>
+  </si>
+  <si>
+    <t>1,736 €</t>
+  </si>
+  <si>
+    <t>2,385 €</t>
+  </si>
+  <si>
+    <t>2,571 €</t>
+  </si>
+  <si>
+    <t>943 €</t>
+  </si>
+  <si>
+    <t>2,518 €</t>
+  </si>
+  <si>
+    <t>1,393 €</t>
+  </si>
+  <si>
+    <t>2,212 €</t>
+  </si>
+  <si>
+    <t>1,715 €</t>
+  </si>
+  <si>
+    <t>1,344 €</t>
+  </si>
+  <si>
+    <t>1,346 €</t>
+  </si>
+  <si>
+    <t>1,250 €</t>
+  </si>
+  <si>
+    <t>1,361 €</t>
+  </si>
+  <si>
+    <t>2,019 €</t>
+  </si>
+  <si>
+    <t>1,930 €</t>
+  </si>
+  <si>
+    <t>2,250 €</t>
+  </si>
+  <si>
+    <t>1,683 €</t>
+  </si>
+  <si>
+    <t>847 €</t>
+  </si>
+  <si>
+    <t>1,738 €</t>
+  </si>
+  <si>
+    <t>991 €</t>
+  </si>
+  <si>
+    <t>1,244 €</t>
+  </si>
+  <si>
+    <t>1,650 €</t>
   </si>
   <si>
     <t>1,556 €</t>
@@ -487,127 +604,124 @@
     <t>1,220 €</t>
   </si>
   <si>
-    <t>2,307 €</t>
-  </si>
-  <si>
-    <t>1,000 €</t>
-  </si>
-  <si>
-    <t>1,532 €</t>
-  </si>
-  <si>
-    <t>733 €</t>
-  </si>
-  <si>
-    <t>1,673 €</t>
-  </si>
-  <si>
-    <t>1,800 €</t>
-  </si>
-  <si>
-    <t>1,565 €</t>
-  </si>
-  <si>
-    <t>2,081 €</t>
-  </si>
-  <si>
-    <t>2,697 €</t>
-  </si>
-  <si>
-    <t>1,631 €</t>
-  </si>
-  <si>
-    <t>2,000 €</t>
-  </si>
-  <si>
-    <t>1,667 €</t>
-  </si>
-  <si>
-    <t>1,182 €</t>
-  </si>
-  <si>
-    <t>1,143 €</t>
-  </si>
-  <si>
-    <t>969 €</t>
-  </si>
-  <si>
-    <t>1,285 €</t>
-  </si>
-  <si>
-    <t>1,333 €</t>
-  </si>
-  <si>
-    <t>1,500 €</t>
-  </si>
-  <si>
-    <t>1,708 €</t>
-  </si>
-  <si>
-    <t>2,385 €</t>
-  </si>
-  <si>
-    <t>1,300 €</t>
-  </si>
-  <si>
-    <t>857 €</t>
-  </si>
-  <si>
-    <t>2,245 €</t>
-  </si>
-  <si>
-    <t>2,460 €</t>
-  </si>
-  <si>
-    <t>2,329 €</t>
-  </si>
-  <si>
-    <t>1,709 €</t>
-  </si>
-  <si>
-    <t>3,028 €</t>
-  </si>
-  <si>
-    <t>2,500 €</t>
-  </si>
-  <si>
-    <t>1,843 €</t>
-  </si>
-  <si>
-    <t>943 €</t>
-  </si>
-  <si>
-    <t>1,714 €</t>
-  </si>
-  <si>
-    <t>1,042 €</t>
-  </si>
-  <si>
-    <t>2,273 €</t>
-  </si>
-  <si>
-    <t>1,321 €</t>
-  </si>
-  <si>
-    <t>1,487 €</t>
-  </si>
-  <si>
-    <t>2,285 €</t>
-  </si>
-  <si>
-    <t>1,867 €</t>
-  </si>
-  <si>
-    <t>1,892 €</t>
-  </si>
-  <si>
-    <t>1,599 €</t>
-  </si>
-  <si>
-    <t>1,400 €</t>
-  </si>
-  <si>
-    <t>1,579 €</t>
+    <t>88,000 €</t>
+  </si>
+  <si>
+    <t>275,000 €</t>
+  </si>
+  <si>
+    <t>255,000 €</t>
+  </si>
+  <si>
+    <t>285,000 €</t>
+  </si>
+  <si>
+    <t>155,000 €</t>
+  </si>
+  <si>
+    <t>54,000 €</t>
+  </si>
+  <si>
+    <t>42,000 €</t>
+  </si>
+  <si>
+    <t>190,000 €</t>
+  </si>
+  <si>
+    <t>380,000 €</t>
+  </si>
+  <si>
+    <t>295,000 €</t>
+  </si>
+  <si>
+    <t>158,000 €</t>
+  </si>
+  <si>
+    <t>139,000 €</t>
+  </si>
+  <si>
+    <t>105,000 €</t>
+  </si>
+  <si>
+    <t>154,440 €</t>
+  </si>
+  <si>
+    <t>466,788 €</t>
+  </si>
+  <si>
+    <t>136,056 €</t>
+  </si>
+  <si>
+    <t>109,000 €</t>
+  </si>
+  <si>
+    <t>40,990 €</t>
+  </si>
+  <si>
+    <t>35,990 €</t>
+  </si>
+  <si>
+    <t>39,990 €</t>
+  </si>
+  <si>
+    <t>125,000 €</t>
+  </si>
+  <si>
+    <t>76,320 €</t>
+  </si>
+  <si>
+    <t>61,700 €</t>
+  </si>
+  <si>
+    <t>119,700 €</t>
+  </si>
+  <si>
+    <t>125,900 €</t>
+  </si>
+  <si>
+    <t>144,900 €</t>
+  </si>
+  <si>
+    <t>165,900 €</t>
+  </si>
+  <si>
+    <t>133,770 €</t>
+  </si>
+  <si>
+    <t>69,900 €</t>
+  </si>
+  <si>
+    <t>35,000 €</t>
+  </si>
+  <si>
+    <t>100,000 €</t>
+  </si>
+  <si>
+    <t>83,000 €</t>
+  </si>
+  <si>
+    <t>110,000 €</t>
+  </si>
+  <si>
+    <t>40,000 €</t>
+  </si>
+  <si>
+    <t>135,000 €</t>
+  </si>
+  <si>
+    <t>69,000 €</t>
+  </si>
+  <si>
+    <t>72,000 €</t>
+  </si>
+  <si>
+    <t>36,500 €</t>
+  </si>
+  <si>
+    <t>101,975 €</t>
+  </si>
+  <si>
+    <t>32,990 €</t>
   </si>
   <si>
     <t>51,350 €</t>
@@ -649,136 +763,10 @@
     <t>179,500 €</t>
   </si>
   <si>
-    <t>110,000 €</t>
-  </si>
-  <si>
     <t>144,620 €</t>
   </si>
   <si>
     <t>77,000 €</t>
-  </si>
-  <si>
-    <t>100,000 €</t>
-  </si>
-  <si>
-    <t>89,990 €</t>
-  </si>
-  <si>
-    <t>95,000 €</t>
-  </si>
-  <si>
-    <t>44,000 €</t>
-  </si>
-  <si>
-    <t>251,000 €</t>
-  </si>
-  <si>
-    <t>45,000 €</t>
-  </si>
-  <si>
-    <t>79,800 €</t>
-  </si>
-  <si>
-    <t>179,000 €</t>
-  </si>
-  <si>
-    <t>199,600 €</t>
-  </si>
-  <si>
-    <t>349,000 €</t>
-  </si>
-  <si>
-    <t>124,000 €</t>
-  </si>
-  <si>
-    <t>155,000 €</t>
-  </si>
-  <si>
-    <t>117,000 €</t>
-  </si>
-  <si>
-    <t>94,900 €</t>
-  </si>
-  <si>
-    <t>37,800 €</t>
-  </si>
-  <si>
-    <t>47,555 €</t>
-  </si>
-  <si>
-    <t>39,990 €</t>
-  </si>
-  <si>
-    <t>35,990 €</t>
-  </si>
-  <si>
-    <t>40,990 €</t>
-  </si>
-  <si>
-    <t>93,000 €</t>
-  </si>
-  <si>
-    <t>26,000 €</t>
-  </si>
-  <si>
-    <t>46,300 €</t>
-  </si>
-  <si>
-    <t>91,020 €</t>
-  </si>
-  <si>
-    <t>169,990 €</t>
-  </si>
-  <si>
-    <t>112,800 €</t>
-  </si>
-  <si>
-    <t>330,000 €</t>
-  </si>
-  <si>
-    <t>170,000 €</t>
-  </si>
-  <si>
-    <t>129,000 €</t>
-  </si>
-  <si>
-    <t>119,700 €</t>
-  </si>
-  <si>
-    <t>133,700 €</t>
-  </si>
-  <si>
-    <t>25,000 €</t>
-  </si>
-  <si>
-    <t>175,000 €</t>
-  </si>
-  <si>
-    <t>37,000 €</t>
-  </si>
-  <si>
-    <t>65,000 €</t>
-  </si>
-  <si>
-    <t>56,500 €</t>
-  </si>
-  <si>
-    <t>68,550 €</t>
-  </si>
-  <si>
-    <t>46,683 €</t>
-  </si>
-  <si>
-    <t>111,625 €</t>
-  </si>
-  <si>
-    <t>275,000 €</t>
-  </si>
-  <si>
-    <t>76,990 €</t>
-  </si>
-  <si>
-    <t>60,000 €</t>
   </si>
 </sst>
 </file>
@@ -1182,25 +1170,25 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="H2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1211,25 +1199,25 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>136</v>
       </c>
       <c r="H3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1240,25 +1228,25 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="H4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I4" t="s">
         <v>133</v>
       </c>
       <c r="J4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1266,28 +1254,28 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="H5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I5" t="s">
         <v>133</v>
       </c>
       <c r="J5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1295,28 +1283,28 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="H6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1324,28 +1312,28 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="I7" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1353,28 +1341,28 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H8" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="I8" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1382,28 +1370,28 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="F9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G9">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="H9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1411,28 +1399,28 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>163</v>
+        <v>109</v>
       </c>
       <c r="H10" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I10" t="s">
         <v>133</v>
       </c>
       <c r="J10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1440,28 +1428,28 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="F11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G11">
-        <v>146</v>
+        <v>226</v>
       </c>
       <c r="H11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I11" t="s">
         <v>133</v>
       </c>
       <c r="J11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1469,28 +1457,28 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="F12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G12">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="H12" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="I12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K12" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1498,28 +1486,28 @@
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="F13">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G13">
-        <v>127</v>
+        <v>82</v>
       </c>
       <c r="H13" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="I13" t="s">
         <v>135</v>
       </c>
       <c r="J13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1527,28 +1515,28 @@
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G14">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="H14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="I14" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="J14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1556,28 +1544,28 @@
         <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G15">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H15" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1585,28 +1573,28 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="F16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G16">
-        <v>103</v>
+        <v>180</v>
       </c>
       <c r="H16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I16" t="s">
         <v>133</v>
       </c>
       <c r="J16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K16" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1614,28 +1602,28 @@
         <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F17">
         <v>2</v>
       </c>
       <c r="G17">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="H17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I17" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K17" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1643,28 +1631,28 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="F18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G18">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="H18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I18" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="J18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K18" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1672,28 +1660,28 @@
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="H19" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="I19" t="s">
         <v>135</v>
       </c>
       <c r="J19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K19" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1701,28 +1689,28 @@
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E20" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G20">
-        <v>110</v>
+        <v>24</v>
       </c>
       <c r="H20" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="I20" t="s">
         <v>135</v>
       </c>
       <c r="J20" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="K20" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1730,28 +1718,28 @@
         <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G21">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="H21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I21" t="s">
         <v>135</v>
       </c>
       <c r="J21" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1759,28 +1747,28 @@
         <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G22">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="H22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="I22" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1788,28 +1776,28 @@
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F23">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>150</v>
+        <v>32</v>
       </c>
       <c r="H23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J23" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1817,28 +1805,28 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E24" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F24">
         <v>1</v>
       </c>
       <c r="G24">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H24" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="I24" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1846,28 +1834,28 @@
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G25">
-        <v>51</v>
+        <v>127</v>
       </c>
       <c r="H25" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="I25" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="J25" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1875,28 +1863,28 @@
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E26" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G26">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="H26" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J26" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K26" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1904,28 +1892,28 @@
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E27" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G27">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="H27" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I27" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="J27" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1933,28 +1921,28 @@
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E28" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F28">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G28">
-        <v>214</v>
+        <v>75</v>
       </c>
       <c r="H28" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1962,28 +1950,28 @@
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E29" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F29">
         <v>3</v>
       </c>
       <c r="G29">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="H29" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1991,28 +1979,28 @@
         <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E30" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G30">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="H30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J30" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K30" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -2020,28 +2008,28 @@
         <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E31" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G31">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="H31" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="I31" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J31" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -2049,28 +2037,28 @@
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E32" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F32">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G32">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="H32" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="I32" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J32" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K32" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -2078,28 +2066,28 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E33" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F33">
         <v>3</v>
       </c>
       <c r="G33">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H33" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="I33" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J33" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -2107,28 +2095,28 @@
         <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E34" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G34">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="H34" t="s">
         <v>124</v>
       </c>
       <c r="I34" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J34" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -2136,28 +2124,28 @@
         <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E35" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G35">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="H35" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="I35" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J35" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K35" t="s">
-        <v>229</v>
+        <v>208</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -2165,28 +2153,28 @@
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E36" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G36">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="H36" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="I36" t="s">
         <v>133</v>
       </c>
       <c r="J36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K36" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -2194,28 +2182,28 @@
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E37" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G37">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H37" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="I37" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J37" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="K37" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -2223,28 +2211,28 @@
         <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E38" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="F38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G38">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="H38" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="I38" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J38" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K38" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -2252,28 +2240,28 @@
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E39" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G39">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H39" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="I39" t="s">
         <v>135</v>
       </c>
       <c r="J39" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="K39" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -2281,28 +2269,28 @@
         <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E40" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G40">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="H40" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="I40" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J40" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="K40" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -2310,28 +2298,28 @@
         <v>9</v>
       </c>
       <c r="D41" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E41" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G41">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="H41" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="I41" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J41" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K41" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -2339,28 +2327,28 @@
         <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E42" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="F42">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G42">
-        <v>49</v>
+        <v>110</v>
       </c>
       <c r="H42" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="I42" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J42" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="K42" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -2368,28 +2356,28 @@
         <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E43" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="F43">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G43">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="H43" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="I43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J43" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K43" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -2397,28 +2385,28 @@
         <v>12</v>
       </c>
       <c r="D44" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E44" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="F44">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G44">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="H44" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="I44" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J44" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="K44" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -2426,28 +2414,28 @@
         <v>13</v>
       </c>
       <c r="D45" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E45" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="F45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G45">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="H45" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="I45" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J45" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="K45" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2455,28 +2443,28 @@
         <v>14</v>
       </c>
       <c r="D46" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E46" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="F46">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G46">
-        <v>109</v>
+        <v>30</v>
       </c>
       <c r="H46" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I46" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J46" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="K46" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -2484,28 +2472,28 @@
         <v>15</v>
       </c>
       <c r="D47" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="E47" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="F47">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G47">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="H47" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="I47" t="s">
         <v>135</v>
       </c>
       <c r="J47" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="K47" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -2513,28 +2501,28 @@
         <v>16</v>
       </c>
       <c r="D48" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E48" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="F48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G48">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="H48" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="I48" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J48" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="K48" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -2542,16 +2530,16 @@
         <v>17</v>
       </c>
       <c r="D49" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E49" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F49">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G49">
-        <v>127</v>
+        <v>40</v>
       </c>
       <c r="H49" t="s">
         <v>116</v>
@@ -2560,10 +2548,10 @@
         <v>135</v>
       </c>
       <c r="J49" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="K49" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -2571,28 +2559,28 @@
         <v>18</v>
       </c>
       <c r="D50" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E50" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F50">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G50">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="H50" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="I50" t="s">
         <v>135</v>
       </c>
       <c r="J50" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="K50" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -2600,28 +2588,28 @@
         <v>19</v>
       </c>
       <c r="D51" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E51" t="s">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="F51">
         <v>1</v>
       </c>
       <c r="G51">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="H51" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="I51" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J51" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="K51" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -2629,28 +2617,28 @@
         <v>20</v>
       </c>
       <c r="D52" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E52" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="F52">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G52">
-        <v>77</v>
+        <v>148</v>
       </c>
       <c r="H52" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="I52" t="s">
         <v>135</v>
       </c>
       <c r="J52" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K52" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -2658,28 +2646,28 @@
         <v>21</v>
       </c>
       <c r="D53" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E53" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F53">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G53">
-        <v>28</v>
+        <v>163</v>
       </c>
       <c r="H53" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I53" t="s">
         <v>135</v>
       </c>
       <c r="J53" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K53" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -2687,28 +2675,28 @@
         <v>22</v>
       </c>
       <c r="D54" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E54" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F54">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G54">
-        <v>50</v>
+        <v>146</v>
       </c>
       <c r="H54" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="I54" t="s">
         <v>135</v>
       </c>
       <c r="J54" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="K54" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -2716,28 +2704,28 @@
         <v>23</v>
       </c>
       <c r="D55" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E55" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F55">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G55">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="H55" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="I55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J55" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K55" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -2745,28 +2733,28 @@
         <v>24</v>
       </c>
       <c r="D56" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E56" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F56">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G56">
-        <v>30</v>
+        <v>127</v>
       </c>
       <c r="H56" t="s">
         <v>115</v>
       </c>
       <c r="I56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J56" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="K56" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -2774,28 +2762,28 @@
         <v>25</v>
       </c>
       <c r="D57" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E57" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F57">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G57">
-        <v>25</v>
+        <v>97</v>
       </c>
       <c r="H57" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="I57" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J57" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K57" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -2803,28 +2791,28 @@
         <v>26</v>
       </c>
       <c r="D58" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E58" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="F58">
         <v>3</v>
       </c>
       <c r="G58">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="H58" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="I58" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="J58" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K58" t="s">
-        <v>251</v>
+        <v>228</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -2832,28 +2820,28 @@
         <v>27</v>
       </c>
       <c r="D59" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E59" t="s">
+        <v>105</v>
+      </c>
+      <c r="F59">
+        <v>3</v>
+      </c>
+      <c r="G59">
         <v>103</v>
       </c>
-      <c r="F59">
-        <v>5</v>
-      </c>
-      <c r="G59">
-        <v>172</v>
-      </c>
       <c r="H59" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="I59" t="s">
         <v>135</v>
       </c>
       <c r="J59" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K59" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -2861,28 +2849,28 @@
         <v>28</v>
       </c>
       <c r="D60" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E60" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F60">
         <v>2</v>
       </c>
       <c r="G60">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H60" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="I60" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J60" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K60" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -2890,28 +2878,28 @@
         <v>29</v>
       </c>
       <c r="D61" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E61" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F61">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G61">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="H61" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="I61" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J61" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K61" t="s">
-        <v>254</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update August 2021 Days 1 to 4
</commit_message>
<xml_diff>
--- a/Diena_15_Web_Scraping/riga_center_60.xlsx
+++ b/Diena_15_Web_Scraping/riga_center_60.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="252">
   <si>
     <t>Sludinājumi 	datums</t>
   </si>
@@ -46,211 +46,250 @@
     <t>Cena</t>
   </si>
   <si>
-    <t>3 istabu dzīvoklis Viktora Štama projektētā jūgendstila namā.</t>
-  </si>
-  <si>
-    <t>Laba cena par dzīvokli izcilā vietā. Panorāmas skats no logiem</t>
-  </si>
-  <si>
-    <t>Izbaudiet Rīgas pilsētas dzīvi, atrodoties tās epicentrā - iegād</t>
-  </si>
-  <si>
-    <t>Наслаждайся прелестями городской жизни, находять в ее эпицентре</t>
-  </si>
-  <si>
-    <t>Продается просторная, солнечная с изолированными комнатами кварт</t>
-  </si>
-  <si>
-    <t>Īpašnieks pārdod izremontētu, mēbelētu, gaišu dzīvokli Rīgas cen</t>
-  </si>
-  <si>
-    <t>Divu istabu, ar ērtu plānojumu dzīvoklis, ēkas piektajā stāvā, i</t>
+    <t>Īpašnieks pārdod gaišu, siltu, plašu dzīvokli ar labu skatu uz V</t>
+  </si>
+  <si>
+    <t>Dzīvokli- renovētā ēkā, puspagraba stāvā, Miera ielā 5. Iegādājo</t>
+  </si>
+  <si>
+    <t>3 - istabu dzīvoklis fasādes mājas 2. stāvā ar logiem gan ielas,</t>
+  </si>
+  <si>
+    <t>Ksulains un plašs dzīvoklis "Skanstes Parkā" Dzīvokli var teikt</t>
+  </si>
+  <si>
+    <t>Investīcijas piedāvājums. Ēkas energoefektivitātes sertifikāts A</t>
+  </si>
+  <si>
+    <t>Pārdod vienistabas dzīvoklis centrā, renovētā mājā, 6. stāvā (na</t>
+  </si>
+  <si>
+    <t>Dzīvokli ar plašu balkonu, 2 izolētām istabām un nelielu viesist</t>
+  </si>
+  <si>
+    <t>Pārdodas 3-istabu dzīvokli renovētā ēkā , Miera ielā 5, kur logi</t>
+  </si>
+  <si>
+    <t>Autostāvvieta iekļauta cenā 8000 euro vērtībā Piedāvājumā lie</t>
+  </si>
+  <si>
+    <t>Plašs dzīvoklis renovētā namā - Krišjāņa Valdemāra 69, dzīvoklis</t>
+  </si>
+  <si>
+    <t>Plašs dzīvoklis renovētā pirmskara mūra ēkā. + viesistaba ir</t>
+  </si>
+  <si>
+    <t>Ekskluzīvs dzīvoklis Klusajā centrā. Viens no prestižākajiem Rīg</t>
+  </si>
+  <si>
+    <t>Pārdošanā ekskluzīvs dzīvoklis Klusajā centrā. Dzīvoklim ir perf</t>
+  </si>
+  <si>
+    <t>Tiek pārdots 4 - istabu dzīvoklis renovētā mājā . Viesistaba ap</t>
+  </si>
+  <si>
+    <t>Divu istabu dzīvoklis ar pilnu apdari un iebūvētām mēbelēm, namā</t>
+  </si>
+  <si>
+    <t>Divu istabu dzīvoklis ar balkonu centra namā Aleksandra Čaka 33,</t>
+  </si>
+  <si>
+    <t>Gaišs un plašs 2, 5 istabu dzīvoklis jaunajā projektā Lāčplēša</t>
+  </si>
+  <si>
+    <t>Piedāvājam iegādāties mēbelētu divistabu dzīvokli jaunajā projek</t>
+  </si>
+  <si>
+    <t>Tiek pārdots četristabu dzīvoklis Rīgas centrā, Hanzas ielā 4, p</t>
+  </si>
+  <si>
+    <t>Projekta attīstītājs piedāvā dzīvokli ar pilnu iekšējo apdari, C</t>
+  </si>
+  <si>
+    <t>Jauns mēbelēts divstāvu dzīvoklis ar augstas kvalitātes iekšējo</t>
   </si>
   <si>
     <t>Pārdodu 3-istabu dzīvokli Vesetas ielā 8, vienā no labākajiem sp</t>
   </si>
   <si>
-    <t>3 комнатная квартира в новом проекте Futuris, полностью мебелиро</t>
-  </si>
-  <si>
-    <t>Plašs divu līmeņu dzīvoklis Rīgas centrā ar terasi. Brīnišķ</t>
-  </si>
-  <si>
-    <t>Iebūvēta privātmāja Rīgas centrā ar privāto terasi. Brīnišķ</t>
-  </si>
-  <si>
-    <t>Pārdod mūsdienīgu, gaišu un plašu dzīvokli renovētā dzīvojamā mā</t>
-  </si>
-  <si>
-    <t>Pārdod modernu un mājīgu 2-istabu dzīvokli Brīvības ielā pie Cēs</t>
-  </si>
-  <si>
-    <t>Skaists un gaumīgs 4-istabu dzīvoklis renovētā mājā blakus parka</t>
-  </si>
-  <si>
-    <t>В новом проекте Lofts&amp;rosegold продаём пятикомнатную квартиру со</t>
-  </si>
-  <si>
-    <t>В новом проекте Lofts&amp;rosegold продаём двухкомнатную квартиру с</t>
-  </si>
-  <si>
-    <t>Хозяин продаёт квартиру в тихом центре. Квартира состоит из</t>
-  </si>
-  <si>
-    <t>Īpašnieks samazina cenu un pārdod dzīvokli ar pēlēko apdari reno</t>
-  </si>
-  <si>
-    <t>Стильная и уютная квартира в центре Риги, высокий первый этаж. К</t>
-  </si>
-  <si>
-    <t>Застройщик предлагает Studio квартиру в полностью реконструирова</t>
-  </si>
-  <si>
-    <t>Аренда с правом выкупа. Застройщик предлагает студио типа кв</t>
-  </si>
-  <si>
-    <t>Trīs istabas izolētas kapitālais remonts, studio tipa istaba, ap</t>
-  </si>
-  <si>
-    <t>Земля в собственности + бесплатный паркинг у дома - бонус для кр</t>
-  </si>
-  <si>
-    <t>Уютно , спокойно , красиво , качественно и стабильно , а ещё оче</t>
-  </si>
-  <si>
-    <t>Земля в собственности - В самом центре Риги, рядом с красивым па</t>
-  </si>
-  <si>
-    <t>Saimnieks pārdod lielisku trīs istabu dzīvokli ar kopējo platību</t>
-  </si>
-  <si>
-    <t>Pārdod dzīvokli centrā Elku ielā. Dzīvoklis atrodas renovētas ēk</t>
-  </si>
-  <si>
-    <t>Īpašnieks pārdod tīru, gaišu, siltu 1-ist. dzīvokli pēc mūsdienī</t>
-  </si>
-  <si>
-    <t>Pārdod bez starpniekiem plašu dzīvokli, augstie griesti , 3 ista</t>
-  </si>
-  <si>
-    <t>Nekustamā īpašuma trīs zelta likumi. -Vieta, -Vieta un -Vi</t>
-  </si>
-  <si>
-    <t>Pārdod īpašumu pašā Rīgas centra sirdī. -Skandināvu stilā iekā</t>
-  </si>
-  <si>
-    <t>Квартира с панорамными окнами и прекрасным видом на Межапарк. Те</t>
-  </si>
-  <si>
-    <t>Īpašnieks pārdod lielisku dzīvokli, labā stāvoklī, labā vietā-fa</t>
-  </si>
-  <si>
-    <t>Eleganta , komfortabla četrustāvu māja Rīgas vēsturiskajā centrā</t>
-  </si>
-  <si>
-    <t>Pārdodu mājīgu 2 istabu studio tipa dzīvokli, vēsturiskā (pirms</t>
-  </si>
-  <si>
-    <t>Pārdod dzīvokli centrā, klusā, zaļā vietā, Ieroču ielā. Dzīvok</t>
-  </si>
-  <si>
-    <t>Pārdodu vienistabas dzīvokli ar 3, 40 m augstiem griestiem. At</t>
-  </si>
-  <si>
-    <t>Plašs dzīvoklis Rīgas centrāar zemi īpašumā. Mājā ir lifts. Dzīv</t>
-  </si>
-  <si>
-    <t>Gaišs iekšpagalms. Pārdod dzīvokli ar jauniem stāvvadiem, jauna</t>
-  </si>
-  <si>
-    <t>Pārdod studio tipa dzīvokli renovētā mājā. Pvn iekļauts cenā.</t>
-  </si>
-  <si>
-    <t>Īpašnieks pārdod dzīvokli renovētā namā Rīgas centrā. Dzīvokļa l</t>
-  </si>
-  <si>
-    <t>Tiek pārdots mēbelēts dzīvoklis.</t>
-  </si>
-  <si>
-    <t>Tiek piedāvāts dzīvoklis ar pilno iekšējo apdari un iebūvētām mē</t>
+    <t>Īpašnieks pārdod 3 istabu dzīvokli (visas istabas izolētas), Cen</t>
+  </si>
+  <si>
+    <t>Plašs piecu istabu dzīvoklis prestižā Rīgas rajonā. Kluso ce</t>
+  </si>
+  <si>
+    <t>Tiek pārdots divu līmeņu 4 istabu dzīvoklis Rīgā, Vīlandes ielā</t>
+  </si>
+  <si>
+    <t>Продается 1-комнатная квартира со всеми удобствами. Поставлены с</t>
+  </si>
+  <si>
+    <t>Plašs, pārdomāts studijas tipa dzīvoklis Vecrīgā. Īpašumam 2</t>
+  </si>
+  <si>
+    <t>Дом Сдан В Эксплуатацию . 2-комнатная квартира напрямую от застр</t>
+  </si>
+  <si>
+    <t>Аренда с правом выкупа. Застройщик предлагает 2-х комнатную</t>
+  </si>
+  <si>
+    <t>Augstākās kvalitātes jauns dzīvoklis izsmalcinātā projektā klusa</t>
+  </si>
+  <si>
+    <t>Tiek pārdots divu istabu dzīvoklis Klusajā centrā - Dzirnavu 6.</t>
+  </si>
+  <si>
+    <t>Tiek pārdots 4 istabu dzīvoklis Klusajā centrā - Dzirnavu 6.</t>
+  </si>
+  <si>
+    <t>Pārdod trīsistabu dzīvokli jaunājā projektā preti Viesturdārza p</t>
+  </si>
+  <si>
+    <t>Īpašnieks pārdod plašu trīsistabu dzīvokli Rīgas centrā. Plā</t>
+  </si>
+  <si>
+    <t>3D tūre, izstaigā dzīvokli, esot mājās. Links pievienots zemāk.</t>
+  </si>
+  <si>
+    <t>Pārdošanā dzīvoklis pilnībā renovētā ēkā Rīgas klusajā centrā, s</t>
   </si>
   <si>
     <t>Tiek piedāvāts dzīvoklis bez apdares, kas atrodas Blaumaņa ielā</t>
   </si>
   <si>
-    <t>Īpašnieks pārdod dzīvokli pašā Rīgas centrā - Lāčplēša Pasāžas s</t>
-  </si>
-  <si>
-    <t>Lielisks investīciju objekts, pašā centrā. Dzīvokli iespējams sa</t>
-  </si>
-  <si>
-    <t>Atsevišķi stāvošs divstāvu dzīvoklis ar velvētu 12m2 lielu pagra</t>
-  </si>
-  <si>
-    <t>Labs dzīvoklis labā mājā - projektā "Duntes Ozoli" - vieta auto</t>
-  </si>
-  <si>
-    <t>Pārdodas 3-istabu dzīvokli renovētā ēkā , Miera ielā 5, kur logi</t>
-  </si>
-  <si>
-    <t>Īpašnieks pārdod kapitāli izremontētu divistabu dzīvokli centrā.</t>
-  </si>
-  <si>
-    <t>Lielisks novietojums, saprātīga cena. Pagalma māja ar ieeju no</t>
-  </si>
-  <si>
-    <t>Gogoļa 10</t>
-  </si>
-  <si>
-    <t>Teātra 12</t>
+    <t>Tiek piedāvāts pārdošanai dzīvoklis (platībā 100, 5 m2 – 4 istab</t>
+  </si>
+  <si>
+    <t>5 izolētas istabas, atsevišķa virtuve, 2 san/mezgli. Griestu a</t>
+  </si>
+  <si>
+    <t>Компактная, уютная квартира студийного типа в центральном районе</t>
+  </si>
+  <si>
+    <t>Renovētā koka ēkā tiek piedāvāts 4 istabu dzīvoklis. Dzīvokl</t>
+  </si>
+  <si>
+    <t>Pārdod 2 istabu dzīvokli renovētā koka ēkā. Pārdomāts un ērt</t>
+  </si>
+  <si>
+    <t>Bez starpniekiem. Īpašniece pārdod siltu un mājīgu 1-istabas mēb</t>
+  </si>
+  <si>
+    <t>Divistabu dzīvoklis 1870.gados būvētā koka ēkā, klusā Grīziņkaln</t>
+  </si>
+  <si>
+    <t>Piedāvājam iegādāties 3 istabu dzīvokli Stabu ielā 92, renovētā</t>
+  </si>
+  <si>
+    <t>Autostāvvieta iekļauta cenā ( 8000€ vērtībā) Virtuve iekļauta c</t>
+  </si>
+  <si>
+    <t>Квартира на продажу в новом проекте Park Alley - Rūpniecības 44</t>
+  </si>
+  <si>
+    <t>Projekta attīstītājs piedāvā iegādāties dzīvoklis, kas atrodas p</t>
+  </si>
+  <si>
+    <t>Квартира находится в тихом месте в пешей доступности с старым го</t>
+  </si>
+  <si>
+    <t>Dzīvoklis ar balkonu pievilcīgā vietā, netālu no pilsētas centra</t>
+  </si>
+  <si>
+    <t>Pārdodam plašu 4-istabu dzīvokli Centrā. Trīs izolētas istaba</t>
+  </si>
+  <si>
+    <t>Tiek pārdots divu istabu dzīvoklis pēc nesen veikta remonta, tas</t>
+  </si>
+  <si>
+    <t>Tiek pārdots gaišs un mājīgs 3 istabu dzīvoklis ar 2 guļamistabā</t>
+  </si>
+  <si>
+    <t>Продают , Rīga, Centrs, Rīga, Alauksta 9. Продаётся уютная, акку</t>
+  </si>
+  <si>
+    <t>Pārdod 4 istabu (3 guļamistabas) dzīvokli Skolas ielā 25. Dzīvo</t>
+  </si>
+  <si>
+    <t>Skaists, moderns, pilnībā iekārtots dzīvoklis ar mēbelēm, pēc ne</t>
+  </si>
+  <si>
+    <t>Grīziņkalna Republika ir vieta, kur savu īsto mājokli atradīs ak</t>
+  </si>
+  <si>
+    <t>Редкое предложение , Дешевле на 27% без посредников . Посольский</t>
+  </si>
+  <si>
+    <t>Tiek pārdots 2-istabu dzīvoklis Rīgas centrā. Logi ir pagalm</t>
+  </si>
+  <si>
+    <t>Īpašnieks pārdod dzīvokli renovētā namā. Ēkai veikta vienkāršotā</t>
+  </si>
+  <si>
+    <t>Hanzas 4</t>
+  </si>
+  <si>
+    <t>Miera 5</t>
+  </si>
+  <si>
+    <t>Matīsa 41</t>
+  </si>
+  <si>
+    <t>Grostonas 19</t>
+  </si>
+  <si>
+    <t>Stabu 100</t>
+  </si>
+  <si>
+    <t>Miera 86</t>
+  </si>
+  <si>
+    <t>Ģertrūdes 99</t>
+  </si>
+  <si>
+    <t>Valdemāra 69</t>
+  </si>
+  <si>
+    <t>Bruņinieku 39</t>
+  </si>
+  <si>
+    <t>Ausekļa 5</t>
+  </si>
+  <si>
+    <t>Dzirnavu 6</t>
+  </si>
+  <si>
+    <t>Čaka 33</t>
+  </si>
+  <si>
+    <t>Lāčplēša 11</t>
+  </si>
+  <si>
+    <t>Valdemāra 41A</t>
   </si>
   <si>
     <t>Dzirnavu 83</t>
   </si>
   <si>
-    <t>Dzirnavu 81</t>
-  </si>
-  <si>
-    <t>Zaļā 4</t>
-  </si>
-  <si>
-    <t>Lāčplēša 52</t>
-  </si>
-  <si>
-    <t>Klijānu 6</t>
+    <t>Tērbatas 26A</t>
   </si>
   <si>
     <t>Vesetas 8</t>
   </si>
   <si>
-    <t>Antonijas 16A</t>
-  </si>
-  <si>
-    <t>Indrānu 8</t>
-  </si>
-  <si>
-    <t>Indrānu 5</t>
-  </si>
-  <si>
-    <t>Cēsu 23</t>
-  </si>
-  <si>
-    <t>Brīvības 165</t>
-  </si>
-  <si>
-    <t>Klusā 11</t>
-  </si>
-  <si>
-    <t>Strēlnieku 8</t>
-  </si>
-  <si>
-    <t>Rūpniecības 16/2</t>
-  </si>
-  <si>
-    <t>Merķeļa 7</t>
-  </si>
-  <si>
-    <t>Cēsu 43</t>
+    <t>Stabu 33</t>
+  </si>
+  <si>
+    <t>Vīlandes 5</t>
+  </si>
+  <si>
+    <t>Vīlandes 12</t>
+  </si>
+  <si>
+    <t>Alauksta 21</t>
+  </si>
+  <si>
+    <t>Jēkaba 26/28</t>
   </si>
   <si>
     <t>Lāčplēša 24</t>
@@ -259,85 +298,91 @@
     <t>Birznieka-Upīša 10</t>
   </si>
   <si>
-    <t>Stabu 60</t>
-  </si>
-  <si>
-    <t>Ausekļa 8</t>
-  </si>
-  <si>
-    <t>Ģertrūdes 91</t>
-  </si>
-  <si>
-    <t>Pulkv. Brieža 13</t>
-  </si>
-  <si>
-    <t>Elku 4</t>
-  </si>
-  <si>
-    <t>Tallinas 75A</t>
-  </si>
-  <si>
-    <t>Matīsa 89a</t>
-  </si>
-  <si>
-    <t>Blaumaņa 26</t>
-  </si>
-  <si>
-    <t>Stabu 20</t>
-  </si>
-  <si>
-    <t>Duntes 28</t>
-  </si>
-  <si>
-    <t>Klusā 18</t>
-  </si>
-  <si>
-    <t>Skolas 36a</t>
-  </si>
-  <si>
-    <t>Klusā 9</t>
-  </si>
-  <si>
-    <t>Ieroču 10</t>
-  </si>
-  <si>
-    <t>Kazarmu 3a</t>
-  </si>
-  <si>
-    <t>Brīvības 150</t>
-  </si>
-  <si>
-    <t>Brīvības 39a</t>
-  </si>
-  <si>
-    <t>Avotu 4</t>
-  </si>
-  <si>
-    <t>Katrīnas d. 26</t>
-  </si>
-  <si>
-    <t>Blaumaņa 9A</t>
+    <t>Mednieku 5</t>
+  </si>
+  <si>
+    <t>Rūpniecības 50</t>
+  </si>
+  <si>
+    <t>Lāčplēša 47</t>
+  </si>
+  <si>
+    <t>Krasta 11</t>
+  </si>
+  <si>
+    <t>Valdemāra 23</t>
   </si>
   <si>
     <t>Blaumaņa 9</t>
   </si>
   <si>
-    <t>Lāčplēša 43</t>
-  </si>
-  <si>
-    <t>Blaumaņa 27</t>
-  </si>
-  <si>
-    <t>Čaka 105</t>
-  </si>
-  <si>
-    <t>Miera 5</t>
-  </si>
-  <si>
-    <t>Ģertrūdes 110</t>
-  </si>
-  <si>
-    <t>Tērbatas 41/43</t>
+    <t>Merķeļa 6</t>
+  </si>
+  <si>
+    <t>Elijas 5</t>
+  </si>
+  <si>
+    <t>Pērnavas 39</t>
+  </si>
+  <si>
+    <t>Artilērijas 71</t>
+  </si>
+  <si>
+    <t>Čaka 151</t>
+  </si>
+  <si>
+    <t>Krāsotāju 15B</t>
+  </si>
+  <si>
+    <t>Stabu 92</t>
+  </si>
+  <si>
+    <t>Rūpniecības 44</t>
+  </si>
+  <si>
+    <t>M. Piena 6</t>
+  </si>
+  <si>
+    <t>J. Daliņa 4</t>
+  </si>
+  <si>
+    <t>Sadovņikova 18</t>
+  </si>
+  <si>
+    <t>Valdemāra 159</t>
+  </si>
+  <si>
+    <t>Grostonas 25</t>
+  </si>
+  <si>
+    <t>Alauksta 9</t>
+  </si>
+  <si>
+    <t>Skolas 25</t>
+  </si>
+  <si>
+    <t>Asara 12</t>
+  </si>
+  <si>
+    <t>Valdemāra 135</t>
+  </si>
+  <si>
+    <t>6/6</t>
+  </si>
+  <si>
+    <t>1/6</t>
+  </si>
+  <si>
+    <t>2/6</t>
+  </si>
+  <si>
+    <t>5/10</t>
+  </si>
+  <si>
+    <t>2/7</t>
+  </si>
+  <si>
+    <t>4/4</t>
   </si>
   <si>
     <t>2/5</t>
@@ -346,427 +391,385 @@
     <t>6/7</t>
   </si>
   <si>
-    <t>4/7</t>
-  </si>
-  <si>
-    <t>7/7</t>
+    <t>5/7</t>
+  </si>
+  <si>
+    <t>2/8</t>
+  </si>
+  <si>
+    <t>1/8</t>
+  </si>
+  <si>
+    <t>4/6</t>
+  </si>
+  <si>
+    <t>5/6</t>
+  </si>
+  <si>
+    <t>1/5</t>
   </si>
   <si>
     <t>5/5</t>
   </si>
   <si>
-    <t>5/9</t>
-  </si>
-  <si>
-    <t>5/7</t>
-  </si>
-  <si>
-    <t>1/5</t>
-  </si>
-  <si>
-    <t>2/6</t>
-  </si>
-  <si>
-    <t>5/6</t>
+    <t>4/5</t>
+  </si>
+  <si>
+    <t>3/6</t>
+  </si>
+  <si>
+    <t>2/4</t>
+  </si>
+  <si>
+    <t>3/7</t>
+  </si>
+  <si>
+    <t>2/2</t>
+  </si>
+  <si>
+    <t>14/24</t>
   </si>
   <si>
     <t>3/5</t>
   </si>
   <si>
-    <t>4/5</t>
-  </si>
-  <si>
-    <t>4/6</t>
-  </si>
-  <si>
-    <t>3/6</t>
-  </si>
-  <si>
-    <t>1/6</t>
-  </si>
-  <si>
-    <t>3/3</t>
-  </si>
-  <si>
-    <t>6/6</t>
-  </si>
-  <si>
-    <t>11/16</t>
-  </si>
-  <si>
-    <t>3/9</t>
-  </si>
-  <si>
-    <t>2/4</t>
-  </si>
-  <si>
-    <t>3/4</t>
-  </si>
-  <si>
-    <t>4/4</t>
-  </si>
-  <si>
-    <t>2/2</t>
-  </si>
-  <si>
-    <t>3/16</t>
-  </si>
-  <si>
     <t>P. kara</t>
   </si>
   <si>
+    <t>Renov.</t>
+  </si>
+  <si>
     <t>Jaun.</t>
   </si>
   <si>
     <t>Specpr.</t>
   </si>
   <si>
-    <t>Renov.</t>
-  </si>
-  <si>
-    <t>Staļina</t>
-  </si>
-  <si>
     <t>Hrušč.</t>
   </si>
   <si>
-    <t>Priv. m.</t>
-  </si>
-  <si>
-    <t>1,257 €</t>
-  </si>
-  <si>
-    <t>2,022 €</t>
-  </si>
-  <si>
-    <t>3,750 €</t>
-  </si>
-  <si>
-    <t>3,167 €</t>
-  </si>
-  <si>
-    <t>1,649 €</t>
-  </si>
-  <si>
-    <t>3,000 €</t>
-  </si>
-  <si>
-    <t>1,500 €</t>
-  </si>
-  <si>
-    <t>1,610 €</t>
-  </si>
-  <si>
-    <t>3,486 €</t>
-  </si>
-  <si>
-    <t>1,305 €</t>
-  </si>
-  <si>
-    <t>1,756 €</t>
-  </si>
-  <si>
-    <t>1,695 €</t>
-  </si>
-  <si>
-    <t>1,944 €</t>
-  </si>
-  <si>
-    <t>2,206 €</t>
-  </si>
-  <si>
-    <t>2,593 €</t>
-  </si>
-  <si>
-    <t>2,346 €</t>
-  </si>
-  <si>
-    <t>1,879 €</t>
-  </si>
-  <si>
-    <t>1,708 €</t>
-  </si>
-  <si>
-    <t>1,333 €</t>
-  </si>
-  <si>
-    <t>1,736 €</t>
-  </si>
-  <si>
-    <t>2,385 €</t>
-  </si>
-  <si>
-    <t>2,571 €</t>
-  </si>
-  <si>
-    <t>943 €</t>
-  </si>
-  <si>
-    <t>2,518 €</t>
-  </si>
-  <si>
-    <t>1,393 €</t>
-  </si>
-  <si>
-    <t>2,212 €</t>
-  </si>
-  <si>
-    <t>1,715 €</t>
-  </si>
-  <si>
-    <t>1,344 €</t>
-  </si>
-  <si>
-    <t>1,346 €</t>
+    <t>1,404 €</t>
+  </si>
+  <si>
+    <t>897 €</t>
+  </si>
+  <si>
+    <t>1,786 €</t>
+  </si>
+  <si>
+    <t>2,419 €</t>
+  </si>
+  <si>
+    <t>2,239 €</t>
+  </si>
+  <si>
+    <t>1,852 €</t>
+  </si>
+  <si>
+    <t>1,572 €</t>
+  </si>
+  <si>
+    <t>1,891 €</t>
+  </si>
+  <si>
+    <t>1,363 €</t>
+  </si>
+  <si>
+    <t>2,253 €</t>
+  </si>
+  <si>
+    <t>2,961 €</t>
+  </si>
+  <si>
+    <t>2,323 €</t>
+  </si>
+  <si>
+    <t>2,250 €</t>
+  </si>
+  <si>
+    <t>1,700 €</t>
+  </si>
+  <si>
+    <t>3,679 €</t>
+  </si>
+  <si>
+    <t>3,378 €</t>
+  </si>
+  <si>
+    <t>2,136 €</t>
+  </si>
+  <si>
+    <t>3,089 €</t>
+  </si>
+  <si>
+    <t>2,176 €</t>
+  </si>
+  <si>
+    <t>1,678 €</t>
+  </si>
+  <si>
+    <t>1,580 €</t>
+  </si>
+  <si>
+    <t>1,741 €</t>
+  </si>
+  <si>
+    <t>2,792 €</t>
+  </si>
+  <si>
+    <t>1,020 €</t>
+  </si>
+  <si>
+    <t>1,889 €</t>
+  </si>
+  <si>
+    <t>2,225 €</t>
+  </si>
+  <si>
+    <t>2,300 €</t>
+  </si>
+  <si>
+    <t>3,061 €</t>
+  </si>
+  <si>
+    <t>2,500 €</t>
+  </si>
+  <si>
+    <t>2,371 €</t>
+  </si>
+  <si>
+    <t>2,000 €</t>
+  </si>
+  <si>
+    <t>2,233 €</t>
+  </si>
+  <si>
+    <t>1,590 €</t>
+  </si>
+  <si>
+    <t>2,364 €</t>
+  </si>
+  <si>
+    <t>1,294 €</t>
+  </si>
+  <si>
+    <t>1,600 €</t>
+  </si>
+  <si>
+    <t>1,000 €</t>
   </si>
   <si>
     <t>1,250 €</t>
   </si>
   <si>
-    <t>1,361 €</t>
-  </si>
-  <si>
-    <t>2,019 €</t>
-  </si>
-  <si>
-    <t>1,930 €</t>
-  </si>
-  <si>
-    <t>2,250 €</t>
-  </si>
-  <si>
-    <t>1,683 €</t>
-  </si>
-  <si>
-    <t>847 €</t>
-  </si>
-  <si>
-    <t>1,738 €</t>
-  </si>
-  <si>
-    <t>991 €</t>
-  </si>
-  <si>
-    <t>1,244 €</t>
-  </si>
-  <si>
-    <t>1,650 €</t>
-  </si>
-  <si>
-    <t>1,556 €</t>
-  </si>
-  <si>
-    <t>800 €</t>
-  </si>
-  <si>
-    <t>2,035 €</t>
-  </si>
-  <si>
-    <t>2,025 €</t>
-  </si>
-  <si>
-    <t>2,356 €</t>
-  </si>
-  <si>
-    <t>2,045 €</t>
-  </si>
-  <si>
-    <t>2,371 €</t>
-  </si>
-  <si>
-    <t>939 €</t>
-  </si>
-  <si>
-    <t>724 €</t>
-  </si>
-  <si>
-    <t>1,115 €</t>
-  </si>
-  <si>
-    <t>1,563 €</t>
-  </si>
-  <si>
-    <t>1,181 €</t>
-  </si>
-  <si>
-    <t>1,851 €</t>
-  </si>
-  <si>
-    <t>1,618 €</t>
-  </si>
-  <si>
-    <t>1,404 €</t>
-  </si>
-  <si>
-    <t>1,540 €</t>
-  </si>
-  <si>
-    <t>1,220 €</t>
-  </si>
-  <si>
-    <t>88,000 €</t>
+    <t>1,955 €</t>
+  </si>
+  <si>
+    <t>1,885 €</t>
+  </si>
+  <si>
+    <t>1,417 €</t>
+  </si>
+  <si>
+    <t>500 €</t>
+  </si>
+  <si>
+    <t>1,388 €</t>
+  </si>
+  <si>
+    <t>1,684 €</t>
+  </si>
+  <si>
+    <t>2,232 €</t>
+  </si>
+  <si>
+    <t>2,014 €</t>
+  </si>
+  <si>
+    <t>1,424 €</t>
+  </si>
+  <si>
+    <t>1,078 €</t>
+  </si>
+  <si>
+    <t>989 €</t>
+  </si>
+  <si>
+    <t>1,462 €</t>
+  </si>
+  <si>
+    <t>2,523 €</t>
+  </si>
+  <si>
+    <t>1,489 €</t>
+  </si>
+  <si>
+    <t>2,041 €</t>
+  </si>
+  <si>
+    <t>2,317 €</t>
+  </si>
+  <si>
+    <t>1,932 €</t>
+  </si>
+  <si>
+    <t>798 €</t>
+  </si>
+  <si>
+    <t>160,000 €</t>
+  </si>
+  <si>
+    <t>50,220 €</t>
+  </si>
+  <si>
+    <t>125,000 €</t>
+  </si>
+  <si>
+    <t>150,000 €</t>
+  </si>
+  <si>
+    <t>91,800 €</t>
+  </si>
+  <si>
+    <t>50,000 €</t>
+  </si>
+  <si>
+    <t>99,066 €</t>
+  </si>
+  <si>
+    <t>144,620 €</t>
+  </si>
+  <si>
+    <t>107,800 €</t>
+  </si>
+  <si>
+    <t>74,990 €</t>
+  </si>
+  <si>
+    <t>196,000 €</t>
+  </si>
+  <si>
+    <t>450,000 €</t>
+  </si>
+  <si>
+    <t>300,000 €</t>
+  </si>
+  <si>
+    <t>230,000 €</t>
+  </si>
+  <si>
+    <t>72,000 €</t>
+  </si>
+  <si>
+    <t>78,200 €</t>
+  </si>
+  <si>
+    <t>283,270 €</t>
+  </si>
+  <si>
+    <t>220,000 €</t>
+  </si>
+  <si>
+    <t>380,000 €</t>
+  </si>
+  <si>
+    <t>185,000 €</t>
+  </si>
+  <si>
+    <t>198,000 €</t>
+  </si>
+  <si>
+    <t>79,000 €</t>
   </si>
   <si>
     <t>275,000 €</t>
   </si>
   <si>
-    <t>255,000 €</t>
-  </si>
-  <si>
-    <t>285,000 €</t>
-  </si>
-  <si>
-    <t>155,000 €</t>
-  </si>
-  <si>
-    <t>54,000 €</t>
-  </si>
-  <si>
-    <t>42,000 €</t>
+    <t>371,280 €</t>
+  </si>
+  <si>
+    <t>25,500 €</t>
+  </si>
+  <si>
+    <t>102,000 €</t>
+  </si>
+  <si>
+    <t>117,900 €</t>
+  </si>
+  <si>
+    <t>98,900 €</t>
+  </si>
+  <si>
+    <t>416,300 €</t>
+  </si>
+  <si>
+    <t>140,000 €</t>
+  </si>
+  <si>
+    <t>196,500 €</t>
+  </si>
+  <si>
+    <t>109,700 €</t>
+  </si>
+  <si>
+    <t>390,000 €</t>
+  </si>
+  <si>
+    <t>110,000 €</t>
+  </si>
+  <si>
+    <t>30,000 €</t>
+  </si>
+  <si>
+    <t>166,140 €</t>
+  </si>
+  <si>
+    <t>69,730 €</t>
+  </si>
+  <si>
+    <t>34,000 €</t>
+  </si>
+  <si>
+    <t>22,000 €</t>
+  </si>
+  <si>
+    <t>93,000 €</t>
+  </si>
+  <si>
+    <t>112,800 €</t>
+  </si>
+  <si>
+    <t>250,000 €</t>
+  </si>
+  <si>
+    <t>145,000 €</t>
+  </si>
+  <si>
+    <t>76,900 €</t>
+  </si>
+  <si>
+    <t>34,500 €</t>
+  </si>
+  <si>
+    <t>92,000 €</t>
+  </si>
+  <si>
+    <t>76,000 €</t>
+  </si>
+  <si>
+    <t>249,000 €</t>
   </si>
   <si>
     <t>190,000 €</t>
   </si>
   <si>
-    <t>380,000 €</t>
-  </si>
-  <si>
-    <t>295,000 €</t>
-  </si>
-  <si>
-    <t>158,000 €</t>
-  </si>
-  <si>
-    <t>139,000 €</t>
-  </si>
-  <si>
-    <t>105,000 €</t>
-  </si>
-  <si>
-    <t>154,440 €</t>
-  </si>
-  <si>
-    <t>466,788 €</t>
-  </si>
-  <si>
-    <t>136,056 €</t>
-  </si>
-  <si>
-    <t>109,000 €</t>
-  </si>
-  <si>
-    <t>40,990 €</t>
-  </si>
-  <si>
-    <t>35,990 €</t>
-  </si>
-  <si>
-    <t>39,990 €</t>
-  </si>
-  <si>
-    <t>125,000 €</t>
-  </si>
-  <si>
-    <t>76,320 €</t>
-  </si>
-  <si>
-    <t>61,700 €</t>
-  </si>
-  <si>
-    <t>119,700 €</t>
-  </si>
-  <si>
-    <t>125,900 €</t>
-  </si>
-  <si>
-    <t>144,900 €</t>
-  </si>
-  <si>
-    <t>165,900 €</t>
-  </si>
-  <si>
-    <t>133,770 €</t>
-  </si>
-  <si>
-    <t>69,900 €</t>
-  </si>
-  <si>
-    <t>35,000 €</t>
-  </si>
-  <si>
-    <t>100,000 €</t>
-  </si>
-  <si>
-    <t>83,000 €</t>
-  </si>
-  <si>
-    <t>110,000 €</t>
-  </si>
-  <si>
-    <t>40,000 €</t>
-  </si>
-  <si>
-    <t>135,000 €</t>
-  </si>
-  <si>
-    <t>69,000 €</t>
-  </si>
-  <si>
-    <t>72,000 €</t>
-  </si>
-  <si>
-    <t>36,500 €</t>
-  </si>
-  <si>
-    <t>101,975 €</t>
-  </si>
-  <si>
-    <t>32,990 €</t>
-  </si>
-  <si>
-    <t>51,350 €</t>
-  </si>
-  <si>
-    <t>24,000 €</t>
-  </si>
-  <si>
-    <t>81,385 €</t>
-  </si>
-  <si>
-    <t>83,025 €</t>
-  </si>
-  <si>
-    <t>94,235 €</t>
-  </si>
-  <si>
-    <t>81,795 €</t>
-  </si>
-  <si>
-    <t>80,605 €</t>
-  </si>
-  <si>
-    <t>138,923 €</t>
-  </si>
-  <si>
-    <t>118,086 €</t>
-  </si>
-  <si>
-    <t>162,786 €</t>
-  </si>
-  <si>
-    <t>111,000 €</t>
-  </si>
-  <si>
-    <t>150,000 €</t>
-  </si>
-  <si>
-    <t>179,500 €</t>
-  </si>
-  <si>
-    <t>144,620 €</t>
-  </si>
-  <si>
-    <t>77,000 €</t>
+    <t>85,000 €</t>
+  </si>
+  <si>
+    <t>306,000 €</t>
+  </si>
+  <si>
+    <t>39,900 €</t>
   </si>
 </sst>
 </file>
@@ -1170,25 +1173,25 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G2">
-        <v>70</v>
+        <v>114</v>
       </c>
       <c r="H2" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="I2" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="J2" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="K2" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1199,25 +1202,25 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G3">
-        <v>136</v>
+        <v>56</v>
       </c>
       <c r="H3" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="I3" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="J3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="K3" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1228,25 +1231,25 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H4" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="I4" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="J4" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="K4" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1257,25 +1260,25 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="H5" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="I5" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="J5" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="K5" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1286,25 +1289,25 @@
         <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6">
-        <v>94</v>
+        <v>41</v>
       </c>
       <c r="H6" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="I6" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="J6" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="K6" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1315,25 +1318,25 @@
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="I7" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="J7" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="K7" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1344,25 +1347,25 @@
         <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F8">
         <v>2</v>
       </c>
       <c r="G8">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="H8" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I8" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="J8" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="K8" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1373,25 +1376,25 @@
         <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="H9" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="I9" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="J9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K9" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1402,25 +1405,25 @@
         <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="F10">
         <v>3</v>
       </c>
       <c r="G10">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="H10" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="I10" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="J10" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="K10" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1431,25 +1434,25 @@
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="F11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G11">
-        <v>226</v>
+        <v>55</v>
       </c>
       <c r="H11" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="I11" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="J11" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="K11" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1460,25 +1463,25 @@
         <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="F12">
         <v>3</v>
       </c>
       <c r="G12">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H12" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="I12" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="J12" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="K12" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1489,25 +1492,25 @@
         <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="F13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G13">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="H13" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="I13" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="J13" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="K13" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1518,25 +1521,25 @@
         <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G14">
-        <v>54</v>
+        <v>162</v>
       </c>
       <c r="H14" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="I14" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="J14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K14" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1547,25 +1550,25 @@
         <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F15">
         <v>4</v>
       </c>
       <c r="G15">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="H15" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="I15" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="J15" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="K15" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1576,25 +1579,25 @@
         <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F16">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G16">
-        <v>180</v>
+        <v>32</v>
       </c>
       <c r="H16" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="I16" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="J16" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="K16" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1605,25 +1608,25 @@
         <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F17">
         <v>2</v>
       </c>
       <c r="G17">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="H17" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="I17" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="J17" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="K17" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1634,25 +1637,25 @@
         <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="F18">
         <v>2</v>
       </c>
       <c r="G18">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="H18" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="I18" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="J18" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="K18" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1663,25 +1666,25 @@
         <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="H19" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="I19" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="J19" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="K19" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1689,28 +1692,28 @@
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E20" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G20">
-        <v>24</v>
+        <v>103</v>
       </c>
       <c r="H20" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="I20" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="J20" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="K20" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1718,28 +1721,28 @@
         <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G21">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="H21" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="I21" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="J21" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="K21" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1747,28 +1750,28 @@
         <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E22" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="F22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G22">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="H22" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="I22" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="J22" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="K22" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1776,28 +1779,28 @@
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G23">
-        <v>32</v>
+        <v>118</v>
       </c>
       <c r="H23" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="I23" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="J23" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="K23" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1805,28 +1808,28 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E24" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G24">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="H24" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="I24" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="J24" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="K24" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1834,28 +1837,28 @@
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E25" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="F25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G25">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="H25" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="I25" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="J25" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="K25" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1863,28 +1866,28 @@
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E26" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="F26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G26">
-        <v>50</v>
+        <v>133</v>
       </c>
       <c r="H26" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="I26" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="J26" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="K26" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1892,28 +1895,28 @@
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E27" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="F27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G27">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="H27" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="I27" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="J27" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="K27" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1921,28 +1924,28 @@
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E28" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="F28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G28">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="H28" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="I28" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="J28" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="K28" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1950,28 +1953,28 @@
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E29" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="F29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G29">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="H29" t="s">
         <v>117</v>
       </c>
       <c r="I29" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="J29" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="K29" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1979,28 +1982,28 @@
         <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E30" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F30">
         <v>2</v>
       </c>
       <c r="G30">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="H30" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="I30" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="J30" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="K30" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -2008,28 +2011,28 @@
         <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E31" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G31">
-        <v>26</v>
+        <v>136</v>
       </c>
       <c r="H31" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I31" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="J31" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="K31" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -2037,28 +2040,28 @@
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E32" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G32">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="H32" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="I32" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="J32" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="K32" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -2066,28 +2069,28 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E33" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G33">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="H33" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="I33" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="J33" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="K33" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -2095,28 +2098,28 @@
         <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E34" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="F34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G34">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="H34" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="I34" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="J34" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="K34" t="s">
-        <v>227</v>
+        <v>200</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -2124,28 +2127,28 @@
         <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E35" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="F35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G35">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="H35" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="I35" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="J35" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="K35" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -2153,28 +2156,28 @@
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E36" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G36">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="H36" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I36" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="J36" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="K36" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -2182,28 +2185,28 @@
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E37" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="F37">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G37">
-        <v>30</v>
+        <v>165</v>
       </c>
       <c r="H37" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I37" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="J37" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="K37" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -2211,28 +2214,28 @@
         <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E38" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="F38">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G38">
-        <v>60</v>
+        <v>143</v>
       </c>
       <c r="H38" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="I38" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="J38" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="K38" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -2240,28 +2243,28 @@
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E39" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="F39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G39">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="H39" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="I39" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="J39" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="K39" t="s">
-        <v>231</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -2269,28 +2272,28 @@
         <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E40" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F40">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G40">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="H40" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="I40" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="J40" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="K40" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -2298,28 +2301,28 @@
         <v>9</v>
       </c>
       <c r="D41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E41" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F41">
         <v>1</v>
       </c>
       <c r="G41">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H41" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I41" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="J41" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="K41" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -2327,28 +2330,28 @@
         <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E42" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="F42">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G42">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="H42" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="I42" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="J42" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="K42" t="s">
-        <v>212</v>
+        <v>235</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -2356,28 +2359,28 @@
         <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E43" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F43">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G43">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="H43" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="I43" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="J43" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="K43" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -2385,28 +2388,28 @@
         <v>12</v>
       </c>
       <c r="D44" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E44" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="F44">
         <v>1</v>
       </c>
       <c r="G44">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H44" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="I44" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="J44" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="K44" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -2414,28 +2417,28 @@
         <v>13</v>
       </c>
       <c r="D45" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E45" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="F45">
         <v>2</v>
       </c>
       <c r="G45">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="H45" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="I45" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="J45" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="K45" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2443,28 +2446,28 @@
         <v>14</v>
       </c>
       <c r="D46" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E46" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G46">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="H46" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="I46" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="J46" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="K46" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -2472,28 +2475,28 @@
         <v>15</v>
       </c>
       <c r="D47" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E47" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G47">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="H47" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="I47" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="J47" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="K47" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -2501,28 +2504,28 @@
         <v>16</v>
       </c>
       <c r="D48" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E48" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="F48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G48">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="H48" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="I48" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="J48" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="K48" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -2530,28 +2533,28 @@
         <v>17</v>
       </c>
       <c r="D49" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E49" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G49">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="H49" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="I49" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="J49" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="K49" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -2559,28 +2562,28 @@
         <v>18</v>
       </c>
       <c r="D50" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E50" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="F50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G50">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="H50" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="I50" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="J50" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="K50" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -2588,28 +2591,28 @@
         <v>19</v>
       </c>
       <c r="D51" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E51" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="F51">
         <v>1</v>
       </c>
       <c r="G51">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I51" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="J51" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="K51" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -2617,28 +2620,28 @@
         <v>20</v>
       </c>
       <c r="D52" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E52" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="F52">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G52">
-        <v>148</v>
+        <v>93</v>
       </c>
       <c r="H52" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="I52" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="J52" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="K52" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -2646,28 +2649,28 @@
         <v>21</v>
       </c>
       <c r="D53" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="E53" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="F53">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G53">
-        <v>163</v>
+        <v>52</v>
       </c>
       <c r="H53" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="I53" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="J53" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="K53" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -2675,28 +2678,28 @@
         <v>22</v>
       </c>
       <c r="D54" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="E54" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="F54">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G54">
-        <v>146</v>
+        <v>109</v>
       </c>
       <c r="H54" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="I54" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="J54" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="K54" t="s">
-        <v>245</v>
+        <v>222</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -2704,28 +2707,28 @@
         <v>23</v>
       </c>
       <c r="D55" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E55" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="F55">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G55">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="H55" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="I55" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="J55" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="K55" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -2733,25 +2736,25 @@
         <v>24</v>
       </c>
       <c r="D56" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="E56" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="F56">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G56">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="H56" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="I56" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="J56" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="K56" t="s">
         <v>247</v>
@@ -2762,25 +2765,25 @@
         <v>25</v>
       </c>
       <c r="D57" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="E57" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F57">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G57">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="H57" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="I57" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="J57" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="K57" t="s">
         <v>248</v>
@@ -2791,28 +2794,28 @@
         <v>26</v>
       </c>
       <c r="D58" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="E58" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="F58">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G58">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="H58" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I58" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="J58" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="K58" t="s">
-        <v>228</v>
+        <v>249</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -2820,28 +2823,28 @@
         <v>27</v>
       </c>
       <c r="D59" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="E59" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="F59">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G59">
-        <v>103</v>
+        <v>162</v>
       </c>
       <c r="H59" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="I59" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="J59" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="K59" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -2849,10 +2852,10 @@
         <v>28</v>
       </c>
       <c r="D60" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="E60" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="F60">
         <v>2</v>
@@ -2861,16 +2864,16 @@
         <v>50</v>
       </c>
       <c r="H60" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="I60" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="J60" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="K60" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -2878,28 +2881,28 @@
         <v>29</v>
       </c>
       <c r="D61" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E61" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="F61">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G61">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="H61" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="I61" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="J61" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="K61" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>